<commit_message>
spring boot jpa uml 8
</commit_message>
<xml_diff>
--- a/src/BankingSystemJpa/CheckList.xlsx
+++ b/src/BankingSystemJpa/CheckList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>Logger</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Denomination</t>
   </si>
 </sst>
 </file>
@@ -389,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>8</v>
       </c>
@@ -413,8 +416,11 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -433,8 +439,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -453,8 +462,11 @@
       <c r="H3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -473,23 +485,26 @@
       <c r="H4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -508,8 +523,11 @@
       <c r="H8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -528,8 +546,11 @@
       <c r="H9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -547,6 +568,9 @@
       </c>
       <c r="H10" t="s">
         <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mongodb AuditLog MicroServ 1
</commit_message>
<xml_diff>
--- a/src/BankingSystemJpa/CheckList.xlsx
+++ b/src/BankingSystemJpa/CheckList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\trainee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trainee\Documents\workspace-sts-3.9.3.RELEASE\new_Clone\trainingProgram\src\BankingSystemJpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
   <si>
     <t>Logger</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,10 +498,22 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>